<commit_message>
collision detection sort of works in gui
</commit_message>
<xml_diff>
--- a/src/res/floor_maps/grid pixel layout.xlsx
+++ b/src/res/floor_maps/grid pixel layout.xlsx
@@ -29,6 +29,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -46,9 +47,10 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="28"/>
+      <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -71,7 +73,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -83,6 +85,62 @@
       <left style="hair"/>
       <right style="hair"/>
       <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
       <bottom style="hair"/>
       <diagonal/>
     </border>
@@ -112,12 +170,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -129,15 +187,43 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -222,146 +308,197 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="E1:M9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P3" activeCellId="0" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="46.3" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="6" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1" style="1" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.7"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="46.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="n">
+        <v>96</v>
+      </c>
+      <c r="C1" s="2" t="n">
+        <f aca="false">B1+96</f>
+        <v>192</v>
+      </c>
+      <c r="D1" s="2" t="n">
+        <f aca="false">C1+96</f>
+        <v>288</v>
+      </c>
       <c r="E1" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F1" s="3" t="n">
-        <v>96</v>
+        <f aca="false">D1+96</f>
+        <v>384</v>
+      </c>
+      <c r="F1" s="2" t="n">
+        <f aca="false">E1+96</f>
+        <v>480</v>
       </c>
       <c r="G1" s="2" t="n">
         <f aca="false">F1+96</f>
-        <v>192</v>
+        <v>576</v>
       </c>
       <c r="H1" s="2" t="n">
         <f aca="false">G1+96</f>
-        <v>288</v>
+        <v>672</v>
       </c>
       <c r="I1" s="2" t="n">
         <f aca="false">H1+96</f>
-        <v>384</v>
+        <v>768</v>
       </c>
       <c r="J1" s="2" t="n">
         <f aca="false">I1+96</f>
-        <v>480</v>
+        <v>864</v>
       </c>
       <c r="K1" s="2" t="n">
         <f aca="false">J1+96</f>
-        <v>576</v>
+        <v>960</v>
       </c>
       <c r="L1" s="2" t="n">
         <f aca="false">K1+96</f>
-        <v>672</v>
-      </c>
-      <c r="M1" s="4"/>
-    </row>
-    <row r="2" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E2" s="3" t="n">
+        <v>1056</v>
+      </c>
+      <c r="M1" s="2" t="n">
+        <f aca="false">L1+96</f>
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="46.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="4"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
-    </row>
-    <row r="3" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E3" s="6" t="n">
-        <f aca="false">F1+96</f>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="46.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="n">
+        <f aca="false">B1+96</f>
         <v>192</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-    </row>
-    <row r="4" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E4" s="6" t="n">
-        <f aca="false">E3+96</f>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="46.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
+        <f aca="false">A3+96</f>
         <v>288</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E5" s="6" t="n">
-        <f aca="false">E4+96</f>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" customFormat="false" ht="46.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="n">
+        <f aca="false">A4+96</f>
         <v>384</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E6" s="6" t="n">
-        <f aca="false">E5+96</f>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" customFormat="false" ht="46.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
+        <f aca="false">A5+96</f>
         <v>480</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E7" s="6" t="n">
-        <f aca="false">E6+96</f>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" customFormat="false" ht="46.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
+        <f aca="false">A6+96</f>
         <v>576</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E8" s="6" t="n">
-        <f aca="false">E7+96</f>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="46.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="n">
+        <f aca="false">A7+96</f>
         <v>672</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E9" s="7"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+    </row>
+    <row r="9" customFormat="false" ht="46.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>